<commit_message>
delete template data after export
</commit_message>
<xml_diff>
--- a/TemplateData/Templates.xlsx
+++ b/TemplateData/Templates.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="19635" windowHeight="7800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="18705" windowHeight="8400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -1228,13 +1228,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col width="10.8571428571429" customWidth="1" style="1" min="1" max="1"/>
     <col width="9.571428571428569" customWidth="1" style="1" min="2" max="2"/>
@@ -1384,202 +1384,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>GR03-000150-000-000</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>CSGST0</t>
-        </is>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>8383</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>901</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>24351295</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>GA04-000005-000-101</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>152</v>
-      </c>
-      <c r="F4" s="0" t="inlineStr">
-        <is>
-          <t>CSGST0</t>
-        </is>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>8383</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>2584</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>24351295</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>GR03-000192-000-000</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="F5" s="0" t="inlineStr">
-        <is>
-          <t>CSGST0</t>
-        </is>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>8383</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>806</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L5" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>24351295</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GR03-000164-000-000</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>6</v>
-      </c>
-      <c r="E6" t="n">
-        <v>253</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CSGST0</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>20</v>
-      </c>
-      <c r="H6" t="n">
-        <v>8383</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1518</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>24351295</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>